<commit_message>
trying to get sync in order
</commit_message>
<xml_diff>
--- a/tutorials/Tutorial plan.xlsx
+++ b/tutorials/Tutorial plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guiliberali/Google Drive/Teaching/Teaching - BigData 2024/Github/Big-Data-2024/tutorials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{394195E8-F1F5-D44E-915D-C64644EA2D47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F4C8C29-EF3E-754E-BD80-E9CAC5CB2169}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="760" windowWidth="21960" windowHeight="21580" xr2:uid="{16787138-0C24-184A-98B2-327E13C17B03}"/>
+    <workbookView xWindow="72960" yWindow="-7040" windowWidth="21960" windowHeight="21100" xr2:uid="{16787138-0C24-184A-98B2-327E13C17B03}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
   <si>
     <t>Monday</t>
   </si>
@@ -174,6 +174,9 @@
   </si>
   <si>
     <t>Tutorial 2.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -657,7 +660,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="143" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -674,6 +677,11 @@
         <v>16</v>
       </c>
     </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F2" t="s">
+        <v>45</v>
+      </c>
+    </row>
     <row r="4" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B4" s="5" t="s">
         <v>4</v>

</xml_diff>